<commit_message>
actualizacion con las imagenes de fondo
</commit_message>
<xml_diff>
--- a/citas.xlsx
+++ b/citas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,11 +443,28 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>lunes</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>maría</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>lópez</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>